<commit_message>
finished class files and makefile
</commit_message>
<xml_diff>
--- a/Replication.xlsx
+++ b/Replication.xlsx
@@ -5793,15 +5793,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>635000</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>736600</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6191,7 +6191,7 @@
   <dimension ref="A1:C300"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>